<commit_message>
fix diode and last fuse p/n
</commit_message>
<xml_diff>
--- a/hardware/VoltTemp/BOM/VoltTempBOM.xlsx
+++ b/hardware/VoltTemp/BOM/VoltTempBOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lakshaygupta/Documents/LHR/BPS/BPS-VoltTempPCB/hardware/VoltTemp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lakshaygupta/Documents/LHR/BPS/BPS-VoltTempPCB/hardware/VoltTemp/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48FFF331-959B-674B-8E2E-6BEF22545FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC5183B-84AB-284D-886E-F054D0D2860F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16680" xr2:uid="{EDF4FD0D-AE22-AE43-BC42-06DCD891D191}"/>
+    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16620" xr2:uid="{EDF4FD0D-AE22-AE43-BC42-06DCD891D191}"/>
   </bookViews>
   <sheets>
     <sheet name="VoltTempBOM" sheetId="1" r:id="rId1"/>
@@ -193,9 +193,6 @@
     <t>40mA</t>
   </si>
   <si>
-    <t>FUSC1607X75N</t>
-  </si>
-  <si>
     <t>R53,R54,R55,R56,R57,R58,R59,R60</t>
   </si>
   <si>
@@ -304,9 +301,6 @@
     <t>D_Zener_Small</t>
   </si>
   <si>
-    <t>1N448W</t>
-  </si>
-  <si>
     <t>Diode_SMD:D_0805_2012Metric</t>
   </si>
   <si>
@@ -392,6 +386,12 @@
   </si>
   <si>
     <t>27k</t>
+  </si>
+  <si>
+    <t>BZY55C22 RBG</t>
+  </si>
+  <si>
+    <t>PTSLR06036V250</t>
   </si>
 </sst>
 </file>
@@ -1255,7 +1255,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1322,7 +1322,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -1407,7 +1407,7 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
@@ -1543,7 +1543,7 @@
         <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C17" t="s">
         <v>53</v>
@@ -1563,7 +1563,7 @@
         <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>123</v>
       </c>
       <c r="D18" t="s">
         <v>35</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
         <v>58</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>59</v>
-      </c>
-      <c r="C19" t="s">
-        <v>60</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
@@ -1591,13 +1591,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" t="s">
         <v>61</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>62</v>
-      </c>
-      <c r="C20" t="s">
-        <v>63</v>
       </c>
       <c r="D20" t="s">
         <v>14</v>
@@ -1608,16 +1608,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" t="s">
         <v>64</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>65</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>66</v>
-      </c>
-      <c r="D21" t="s">
-        <v>67</v>
       </c>
       <c r="E21">
         <v>2</v>
@@ -1625,13 +1625,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" t="s">
         <v>68</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>69</v>
-      </c>
-      <c r="C22" t="s">
-        <v>70</v>
       </c>
       <c r="D22" t="s">
         <v>14</v>
@@ -1642,16 +1642,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" t="s">
         <v>71</v>
       </c>
-      <c r="B23" t="s">
-        <v>117</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>72</v>
-      </c>
-      <c r="D23" t="s">
-        <v>73</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1659,13 +1659,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" t="s">
         <v>74</v>
-      </c>
-      <c r="B24" t="s">
-        <v>118</v>
-      </c>
-      <c r="C24" t="s">
-        <v>75</v>
       </c>
       <c r="D24" t="s">
         <v>14</v>
@@ -1676,13 +1676,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" t="s">
         <v>76</v>
-      </c>
-      <c r="B25" t="s">
-        <v>119</v>
-      </c>
-      <c r="C25" t="s">
-        <v>77</v>
       </c>
       <c r="D25" t="s">
         <v>14</v>
@@ -1693,13 +1693,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B26">
         <v>120</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D26" t="s">
         <v>14</v>
@@ -1710,13 +1710,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" t="s">
         <v>80</v>
-      </c>
-      <c r="B27" t="s">
-        <v>120</v>
-      </c>
-      <c r="C27" t="s">
-        <v>81</v>
       </c>
       <c r="D27" t="s">
         <v>14</v>
@@ -1727,16 +1727,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" t="s">
         <v>82</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>83</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>84</v>
-      </c>
-      <c r="D28" t="s">
-        <v>85</v>
       </c>
       <c r="E28">
         <v>5</v>
@@ -1744,16 +1744,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" t="s">
         <v>86</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" t="s">
         <v>87</v>
-      </c>
-      <c r="C29" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" t="s">
-        <v>88</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -1761,16 +1761,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" t="s">
         <v>89</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" t="s">
         <v>90</v>
-      </c>
-      <c r="C30" t="s">
-        <v>90</v>
-      </c>
-      <c r="D30" t="s">
-        <v>91</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1778,16 +1778,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" t="s">
         <v>92</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" t="s">
         <v>93</v>
-      </c>
-      <c r="C31" t="s">
-        <v>94</v>
-      </c>
-      <c r="D31" t="s">
-        <v>95</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -1795,16 +1795,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" t="s">
         <v>96</v>
       </c>
-      <c r="B32" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" t="s">
-        <v>98</v>
-      </c>
       <c r="D32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" t="s">
         <v>99</v>
-      </c>
-      <c r="B33" t="s">
-        <v>100</v>
-      </c>
-      <c r="C33" t="s">
-        <v>101</v>
       </c>
       <c r="D33" t="s">
         <v>46</v>
@@ -1829,16 +1829,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C34">
         <v>1053132104</v>
       </c>
       <c r="D34" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E34">
         <v>4</v>
@@ -1846,16 +1846,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C35">
         <v>1053131107</v>
       </c>
       <c r="D35" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -1863,16 +1863,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B36" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C36">
         <v>1053131106</v>
       </c>
       <c r="D36" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -1880,16 +1880,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C37">
         <v>1053131103</v>
       </c>
       <c r="D37" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -1897,13 +1897,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>112</v>
+      </c>
+      <c r="B38" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" t="s">
         <v>114</v>
-      </c>
-      <c r="B38" t="s">
-        <v>115</v>
-      </c>
-      <c r="D38" t="s">
-        <v>116</v>
       </c>
       <c r="E38">
         <v>8</v>

</xml_diff>

<commit_message>
fix diode and last fuse p/n (#4)
</commit_message>
<xml_diff>
--- a/hardware/VoltTemp/BOM/VoltTempBOM.xlsx
+++ b/hardware/VoltTemp/BOM/VoltTempBOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lakshaygupta/Documents/LHR/BPS/BPS-VoltTempPCB/hardware/VoltTemp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lakshaygupta/Documents/LHR/BPS/BPS-VoltTempPCB/hardware/VoltTemp/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48FFF331-959B-674B-8E2E-6BEF22545FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC5183B-84AB-284D-886E-F054D0D2860F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16680" xr2:uid="{EDF4FD0D-AE22-AE43-BC42-06DCD891D191}"/>
+    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16620" xr2:uid="{EDF4FD0D-AE22-AE43-BC42-06DCD891D191}"/>
   </bookViews>
   <sheets>
     <sheet name="VoltTempBOM" sheetId="1" r:id="rId1"/>
@@ -193,9 +193,6 @@
     <t>40mA</t>
   </si>
   <si>
-    <t>FUSC1607X75N</t>
-  </si>
-  <si>
     <t>R53,R54,R55,R56,R57,R58,R59,R60</t>
   </si>
   <si>
@@ -304,9 +301,6 @@
     <t>D_Zener_Small</t>
   </si>
   <si>
-    <t>1N448W</t>
-  </si>
-  <si>
     <t>Diode_SMD:D_0805_2012Metric</t>
   </si>
   <si>
@@ -392,6 +386,12 @@
   </si>
   <si>
     <t>27k</t>
+  </si>
+  <si>
+    <t>BZY55C22 RBG</t>
+  </si>
+  <si>
+    <t>PTSLR06036V250</t>
   </si>
 </sst>
 </file>
@@ -1255,7 +1255,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1322,7 +1322,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -1407,7 +1407,7 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
@@ -1543,7 +1543,7 @@
         <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C17" t="s">
         <v>53</v>
@@ -1563,7 +1563,7 @@
         <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>123</v>
       </c>
       <c r="D18" t="s">
         <v>35</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
         <v>58</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>59</v>
-      </c>
-      <c r="C19" t="s">
-        <v>60</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
@@ -1591,13 +1591,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" t="s">
         <v>61</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>62</v>
-      </c>
-      <c r="C20" t="s">
-        <v>63</v>
       </c>
       <c r="D20" t="s">
         <v>14</v>
@@ -1608,16 +1608,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" t="s">
         <v>64</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>65</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>66</v>
-      </c>
-      <c r="D21" t="s">
-        <v>67</v>
       </c>
       <c r="E21">
         <v>2</v>
@@ -1625,13 +1625,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" t="s">
         <v>68</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>69</v>
-      </c>
-      <c r="C22" t="s">
-        <v>70</v>
       </c>
       <c r="D22" t="s">
         <v>14</v>
@@ -1642,16 +1642,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" t="s">
         <v>71</v>
       </c>
-      <c r="B23" t="s">
-        <v>117</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>72</v>
-      </c>
-      <c r="D23" t="s">
-        <v>73</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1659,13 +1659,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" t="s">
         <v>74</v>
-      </c>
-      <c r="B24" t="s">
-        <v>118</v>
-      </c>
-      <c r="C24" t="s">
-        <v>75</v>
       </c>
       <c r="D24" t="s">
         <v>14</v>
@@ -1676,13 +1676,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" t="s">
         <v>76</v>
-      </c>
-      <c r="B25" t="s">
-        <v>119</v>
-      </c>
-      <c r="C25" t="s">
-        <v>77</v>
       </c>
       <c r="D25" t="s">
         <v>14</v>
@@ -1693,13 +1693,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B26">
         <v>120</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D26" t="s">
         <v>14</v>
@@ -1710,13 +1710,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" t="s">
         <v>80</v>
-      </c>
-      <c r="B27" t="s">
-        <v>120</v>
-      </c>
-      <c r="C27" t="s">
-        <v>81</v>
       </c>
       <c r="D27" t="s">
         <v>14</v>
@@ -1727,16 +1727,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" t="s">
         <v>82</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>83</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>84</v>
-      </c>
-      <c r="D28" t="s">
-        <v>85</v>
       </c>
       <c r="E28">
         <v>5</v>
@@ -1744,16 +1744,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" t="s">
         <v>86</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" t="s">
         <v>87</v>
-      </c>
-      <c r="C29" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" t="s">
-        <v>88</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -1761,16 +1761,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" t="s">
         <v>89</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" t="s">
         <v>90</v>
-      </c>
-      <c r="C30" t="s">
-        <v>90</v>
-      </c>
-      <c r="D30" t="s">
-        <v>91</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1778,16 +1778,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" t="s">
         <v>92</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" t="s">
         <v>93</v>
-      </c>
-      <c r="C31" t="s">
-        <v>94</v>
-      </c>
-      <c r="D31" t="s">
-        <v>95</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -1795,16 +1795,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" t="s">
         <v>96</v>
       </c>
-      <c r="B32" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" t="s">
-        <v>98</v>
-      </c>
       <c r="D32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1812,13 +1812,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" t="s">
         <v>99</v>
-      </c>
-      <c r="B33" t="s">
-        <v>100</v>
-      </c>
-      <c r="C33" t="s">
-        <v>101</v>
       </c>
       <c r="D33" t="s">
         <v>46</v>
@@ -1829,16 +1829,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C34">
         <v>1053132104</v>
       </c>
       <c r="D34" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E34">
         <v>4</v>
@@ -1846,16 +1846,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C35">
         <v>1053131107</v>
       </c>
       <c r="D35" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -1863,16 +1863,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B36" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C36">
         <v>1053131106</v>
       </c>
       <c r="D36" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -1880,16 +1880,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C37">
         <v>1053131103</v>
       </c>
       <c r="D37" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -1897,13 +1897,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>112</v>
+      </c>
+      <c r="B38" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" t="s">
         <v>114</v>
-      </c>
-      <c r="B38" t="s">
-        <v>115</v>
-      </c>
-      <c r="D38" t="s">
-        <v>116</v>
       </c>
       <c r="E38">
         <v>8</v>

</xml_diff>